<commit_message>
changes for Item rarity and so on
</commit_message>
<xml_diff>
--- a/Srpg_drops.xlsx
+++ b/Srpg_drops.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\Unity3d\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\Unity3d\Projects\ProjectRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,26 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
-  <si>
-    <t>ItemObject</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Jewelery</t>
   </si>
   <si>
-    <t xml:space="preserve">Armor </t>
-  </si>
-  <si>
-    <t>Weapon</t>
-  </si>
-  <si>
     <t xml:space="preserve">Droploot </t>
   </si>
   <si>
-    <t>ItemType</t>
-  </si>
-  <si>
     <t>Ring</t>
   </si>
   <si>
@@ -90,9 +78,6 @@
     <t xml:space="preserve">1 Suffix </t>
   </si>
   <si>
-    <t>Rarity roll</t>
-  </si>
-  <si>
     <t>5 no drop</t>
   </si>
   <si>
@@ -174,9 +159,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>base warponstat per item</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -193,6 +175,45 @@
   </si>
   <si>
     <t>Value * round((Itemlevel+Stage)/2)) * rand[0.8,1.2]</t>
+  </si>
+  <si>
+    <t>ItemObjects</t>
+  </si>
+  <si>
+    <t>ItemTypes</t>
+  </si>
+  <si>
+    <t>Consumable</t>
+  </si>
+  <si>
+    <t>Equip</t>
+  </si>
+  <si>
+    <t>Quest</t>
+  </si>
+  <si>
+    <t>GearTypes</t>
+  </si>
+  <si>
+    <t>INTERN!!!</t>
+  </si>
+  <si>
+    <t>Rarity roll INTERN!!!!!</t>
+  </si>
+  <si>
+    <t>Armor Loot</t>
+  </si>
+  <si>
+    <t>WeaponLoot</t>
+  </si>
+  <si>
+    <t>(BaseSuffixStats)</t>
+  </si>
+  <si>
+    <t>per item(BaseStats)</t>
+  </si>
+  <si>
+    <t>base weaponstat</t>
   </si>
 </sst>
 </file>
@@ -532,282 +553,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="1" t="s">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="1" t="s">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="1" t="s">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="F20" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+      <c r="F21" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="G19" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="B27" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
-        <v>52</v>
-      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F33" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>